<commit_message>
Fixed situation number for Bermude cultivar
</commit_message>
<xml_diff>
--- a/data/protocol_descr_french_Bermude_template.xlsx
+++ b/data/protocol_descr_french_Bermude_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20398"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E1434A-92B6-4DF5-B467-0B17153B996D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3616D437-E679-48F7-9B68-0B4B8A2BFEEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10905" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -852,7 +852,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A36"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,177 +871,177 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>